<commit_message>
Updated Final Tuning Results
</commit_message>
<xml_diff>
--- a/xgb_results_lasso_SMOTE.xlsx
+++ b/xgb_results_lasso_SMOTE.xlsx
@@ -471,16 +471,16 @@
         <v>19</v>
       </c>
       <c r="D2">
-        <v>0.662</v>
+        <v>0.671</v>
       </c>
       <c r="E2">
-        <v>0.583</v>
+        <v>0.599</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G2">
-        <v>0.5682792406613595</v>
+        <v>0.5590936925903246</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -494,16 +494,16 @@
         <v>19</v>
       </c>
       <c r="D3">
-        <v>0.694</v>
+        <v>0.699</v>
       </c>
       <c r="E3">
-        <v>0.605</v>
+        <v>0.621</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G3">
-        <v>0.4807103490508267</v>
+        <v>0.5600122473974281</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -517,16 +517,16 @@
         <v>19</v>
       </c>
       <c r="D4">
-        <v>0.716</v>
+        <v>0.717</v>
       </c>
       <c r="E4">
-        <v>0.619</v>
+        <v>0.627</v>
       </c>
       <c r="F4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4">
-        <v>0.5826699326393141</v>
+        <v>0.629210042865891</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -540,16 +540,16 @@
         <v>19</v>
       </c>
       <c r="D5">
-        <v>0.73</v>
+        <v>0.732</v>
       </c>
       <c r="E5">
-        <v>0.619</v>
+        <v>0.629</v>
       </c>
       <c r="F5">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G5">
-        <v>0.5483772198407838</v>
+        <v>0.5731781996325781</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -563,16 +563,16 @@
         <v>19</v>
       </c>
       <c r="D6">
-        <v>0.6899999999999999</v>
+        <v>0.68</v>
       </c>
       <c r="E6">
-        <v>0.604</v>
+        <v>0.605</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G6">
-        <v>0.5333741579914268</v>
+        <v>0.5364360073484384</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -586,16 +586,16 @@
         <v>19</v>
       </c>
       <c r="D7">
-        <v>0.713</v>
+        <v>0.71</v>
       </c>
       <c r="E7">
-        <v>0.617</v>
+        <v>0.621</v>
       </c>
       <c r="F7">
         <v>8</v>
       </c>
       <c r="G7">
-        <v>0.5903245560318432</v>
+        <v>0.5290875688916106</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -609,16 +609,16 @@
         <v>19</v>
       </c>
       <c r="D8">
-        <v>0.739</v>
+        <v>0.722</v>
       </c>
       <c r="E8">
-        <v>0.619</v>
+        <v>0.629</v>
       </c>
       <c r="F8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G8">
-        <v>0.5480710349050827</v>
+        <v>0.6175750153092467</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -632,16 +632,16 @@
         <v>19</v>
       </c>
       <c r="D9">
-        <v>0.757</v>
+        <v>0.744</v>
       </c>
       <c r="E9">
-        <v>0.627</v>
+        <v>0.633</v>
       </c>
       <c r="F9">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9">
-        <v>0.546846295162278</v>
+        <v>0.5930802204531537</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -655,16 +655,16 @@
         <v>19</v>
       </c>
       <c r="D10">
-        <v>0.6889999999999999</v>
+        <v>0.694</v>
       </c>
       <c r="E10">
-        <v>0.603</v>
+        <v>0.616</v>
       </c>
       <c r="F10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G10">
-        <v>0.545009185548071</v>
+        <v>0.5263319044703001</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -678,16 +678,16 @@
         <v>19</v>
       </c>
       <c r="D11">
-        <v>0.717</v>
+        <v>0.712</v>
       </c>
       <c r="E11">
-        <v>0.619</v>
+        <v>0.623</v>
       </c>
       <c r="F11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11">
-        <v>0.5425597060624617</v>
+        <v>0.5835884874464177</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -701,16 +701,16 @@
         <v>19</v>
       </c>
       <c r="D12">
-        <v>0.746</v>
+        <v>0.727</v>
       </c>
       <c r="E12">
-        <v>0.623</v>
+        <v>0.633</v>
       </c>
       <c r="F12">
         <v>13</v>
       </c>
       <c r="G12">
-        <v>0.5496019595835885</v>
+        <v>0.6313533374157991</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -724,16 +724,16 @@
         <v>19</v>
       </c>
       <c r="D13">
-        <v>0.772</v>
+        <v>0.75</v>
       </c>
       <c r="E13">
-        <v>0.631</v>
+        <v>0.635</v>
       </c>
       <c r="F13">
         <v>19</v>
       </c>
       <c r="G13">
-        <v>0.5480710349050827</v>
+        <v>0.5783833435394978</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -747,16 +747,16 @@
         <v>19</v>
       </c>
       <c r="D14">
-        <v>0.706</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="E14">
-        <v>0.616</v>
+        <v>0.614</v>
       </c>
       <c r="F14">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G14">
-        <v>0.5254133496631965</v>
+        <v>0.5554194733619106</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -770,7 +770,7 @@
         <v>19</v>
       </c>
       <c r="D15">
-        <v>0.725</v>
+        <v>0.712</v>
       </c>
       <c r="E15">
         <v>0.623</v>
@@ -779,7 +779,7 @@
         <v>9</v>
       </c>
       <c r="G15">
-        <v>0.5183710961420698</v>
+        <v>0.5315370483772198</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -793,16 +793,16 @@
         <v>19</v>
       </c>
       <c r="D16">
-        <v>0.76</v>
+        <v>0.736</v>
       </c>
       <c r="E16">
-        <v>0.626</v>
+        <v>0.634</v>
       </c>
       <c r="F16">
         <v>14</v>
       </c>
       <c r="G16">
-        <v>0.5275566442131047</v>
+        <v>0.5627679118187385</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -816,16 +816,16 @@
         <v>19</v>
       </c>
       <c r="D17">
-        <v>0.783</v>
+        <v>0.754</v>
       </c>
       <c r="E17">
-        <v>0.634</v>
+        <v>0.638</v>
       </c>
       <c r="F17">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G17">
-        <v>0.5330679730557256</v>
+        <v>0.5774647887323944</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -839,16 +839,16 @@
         <v>19</v>
       </c>
       <c r="D18">
-        <v>0.715</v>
+        <v>0.701</v>
       </c>
       <c r="E18">
-        <v>0.622</v>
+        <v>0.623</v>
       </c>
       <c r="F18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G18">
-        <v>0.5725658297611758</v>
+        <v>0.5759338640538886</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -865,13 +865,13 @@
         <v>0.73</v>
       </c>
       <c r="E19">
-        <v>0.624</v>
+        <v>0.627</v>
       </c>
       <c r="F19">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>0.5401102265768524</v>
+        <v>0.5202082057562768</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -885,16 +885,16 @@
         <v>19</v>
       </c>
       <c r="D20">
-        <v>0.765</v>
+        <v>0.743</v>
       </c>
       <c r="E20">
-        <v>0.628</v>
+        <v>0.636</v>
       </c>
       <c r="F20">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G20">
-        <v>0.5189834660134721</v>
+        <v>0.6062461726883037</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -908,16 +908,16 @@
         <v>19</v>
       </c>
       <c r="D21">
-        <v>0.786</v>
+        <v>0.762</v>
       </c>
       <c r="E21">
-        <v>0.637</v>
+        <v>0.642</v>
       </c>
       <c r="F21">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G21">
-        <v>0.533680342927128</v>
+        <v>0.580526638089406</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -931,16 +931,16 @@
         <v>19</v>
       </c>
       <c r="D22">
-        <v>0.731</v>
+        <v>0.717</v>
       </c>
       <c r="E22">
-        <v>0.626</v>
+        <v>0.627</v>
       </c>
       <c r="F22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G22">
-        <v>0.5324556031843233</v>
+        <v>0.5569503980404165</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -954,16 +954,16 @@
         <v>19</v>
       </c>
       <c r="D23">
-        <v>0.746</v>
+        <v>0.735</v>
       </c>
       <c r="E23">
-        <v>0.628</v>
+        <v>0.633</v>
       </c>
       <c r="F23">
         <v>11</v>
       </c>
       <c r="G23">
-        <v>0.5208205756276791</v>
+        <v>0.5535823637477036</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -977,16 +977,16 @@
         <v>19</v>
       </c>
       <c r="D24">
-        <v>0.767</v>
+        <v>0.755</v>
       </c>
       <c r="E24">
-        <v>0.629</v>
+        <v>0.643</v>
       </c>
       <c r="F24">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G24">
-        <v>0.5223515003061849</v>
+        <v>0.5970606246172688</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1000,16 +1000,16 @@
         <v>19</v>
       </c>
       <c r="D25">
-        <v>0.795</v>
+        <v>0.77</v>
       </c>
       <c r="E25">
-        <v>0.636</v>
+        <v>0.644</v>
       </c>
       <c r="F25">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G25">
-        <v>0.5342927127985303</v>
+        <v>0.5725658297611758</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1023,16 +1023,16 @@
         <v>19</v>
       </c>
       <c r="D26">
-        <v>0.732</v>
+        <v>0.722</v>
       </c>
       <c r="E26">
-        <v>0.625</v>
+        <v>0.63</v>
       </c>
       <c r="F26">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G26">
-        <v>0.5251071647274954</v>
+        <v>0.5731781996325781</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1046,16 +1046,16 @@
         <v>19</v>
       </c>
       <c r="D27">
-        <v>0.751</v>
+        <v>0.742</v>
       </c>
       <c r="E27">
-        <v>0.629</v>
+        <v>0.639</v>
       </c>
       <c r="F27">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G27">
-        <v>0.524188609920392</v>
+        <v>0.5496019595835885</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1069,16 +1069,16 @@
         <v>19</v>
       </c>
       <c r="D28">
-        <v>0.775</v>
+        <v>0.76</v>
       </c>
       <c r="E28">
-        <v>0.635</v>
+        <v>0.643</v>
       </c>
       <c r="F28">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G28">
-        <v>0.5235762400489896</v>
+        <v>0.5946111451316595</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1092,16 +1092,16 @@
         <v>19</v>
       </c>
       <c r="D29">
-        <v>0.802</v>
+        <v>0.774</v>
       </c>
       <c r="E29">
-        <v>0.636</v>
+        <v>0.645</v>
       </c>
       <c r="F29">
         <v>27</v>
       </c>
       <c r="G29">
-        <v>0.5257195345988978</v>
+        <v>0.575015309246785</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1115,7 +1115,7 @@
         <v>19</v>
       </c>
       <c r="D30">
-        <v>0.737</v>
+        <v>0.727</v>
       </c>
       <c r="E30">
         <v>0.628</v>
@@ -1124,7 +1124,7 @@
         <v>8</v>
       </c>
       <c r="G30">
-        <v>0.5480710349050827</v>
+        <v>0.5759338640538886</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1138,16 +1138,16 @@
         <v>19</v>
       </c>
       <c r="D31">
-        <v>0.759</v>
+        <v>0.743</v>
       </c>
       <c r="E31">
-        <v>0.632</v>
+        <v>0.639</v>
       </c>
       <c r="F31">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G31">
-        <v>0.5315370483772198</v>
+        <v>0.5673606858542559</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1161,16 +1161,16 @@
         <v>19</v>
       </c>
       <c r="D32">
-        <v>0.778</v>
+        <v>0.764</v>
       </c>
       <c r="E32">
-        <v>0.635</v>
+        <v>0.646</v>
       </c>
       <c r="F32">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G32">
-        <v>0.5174525413349663</v>
+        <v>0.5780771586037967</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1184,16 +1184,16 @@
         <v>19</v>
       </c>
       <c r="D33">
-        <v>0.8090000000000001</v>
+        <v>0.781</v>
       </c>
       <c r="E33">
-        <v>0.64</v>
+        <v>0.649</v>
       </c>
       <c r="F33">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G33">
-        <v>0.5202082057562768</v>
+        <v>0.5688916105327618</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1207,16 +1207,16 @@
         <v>19</v>
       </c>
       <c r="D34">
-        <v>0.738</v>
+        <v>0.73</v>
       </c>
       <c r="E34">
-        <v>0.63</v>
+        <v>0.635</v>
       </c>
       <c r="F34">
         <v>8</v>
       </c>
       <c r="G34">
-        <v>0.5554194733619106</v>
+        <v>0.5740967544396816</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1230,16 +1230,16 @@
         <v>19</v>
       </c>
       <c r="D35">
-        <v>0.759</v>
+        <v>0.751</v>
       </c>
       <c r="E35">
-        <v>0.633</v>
+        <v>0.643</v>
       </c>
       <c r="F35">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G35">
-        <v>0.5284751990202082</v>
+        <v>0.5673606858542559</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1253,16 +1253,16 @@
         <v>19</v>
       </c>
       <c r="D36">
-        <v>0.784</v>
+        <v>0.767</v>
       </c>
       <c r="E36">
-        <v>0.638</v>
+        <v>0.647</v>
       </c>
       <c r="F36">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G36">
-        <v>0.522657685241886</v>
+        <v>0.5832823025107164</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1276,16 +1276,16 @@
         <v>19</v>
       </c>
       <c r="D37">
-        <v>0.8159999999999999</v>
+        <v>0.787</v>
       </c>
       <c r="E37">
-        <v>0.64</v>
+        <v>0.653</v>
       </c>
       <c r="F37">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G37">
-        <v>0.5122473974280466</v>
+        <v>0.5673606858542559</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1299,16 +1299,16 @@
         <v>19</v>
       </c>
       <c r="D38">
-        <v>0.751</v>
+        <v>0.736</v>
       </c>
       <c r="E38">
-        <v>0.629</v>
+        <v>0.635</v>
       </c>
       <c r="F38">
         <v>9</v>
       </c>
       <c r="G38">
-        <v>0.5370483772198408</v>
+        <v>0.5808328230251072</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1322,16 +1322,16 @@
         <v>19</v>
       </c>
       <c r="D39">
-        <v>0.776</v>
+        <v>0.756</v>
       </c>
       <c r="E39">
-        <v>0.637</v>
+        <v>0.644</v>
       </c>
       <c r="F39">
         <v>16</v>
       </c>
       <c r="G39">
-        <v>0.530006123698714</v>
+        <v>0.5646050214329456</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1345,16 +1345,16 @@
         <v>19</v>
       </c>
       <c r="D40">
-        <v>0.792</v>
+        <v>0.775</v>
       </c>
       <c r="E40">
-        <v>0.642</v>
+        <v>0.649</v>
       </c>
       <c r="F40">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G40">
-        <v>0.5205143906919779</v>
+        <v>0.5802204531537049</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1368,16 +1368,16 @@
         <v>19</v>
       </c>
       <c r="D41">
-        <v>0.819</v>
+        <v>0.795</v>
       </c>
       <c r="E41">
-        <v>0.642</v>
+        <v>0.653</v>
       </c>
       <c r="F41">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G41">
-        <v>0.5082669932639314</v>
+        <v>0.5621555419473362</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1391,16 +1391,16 @@
         <v>19</v>
       </c>
       <c r="D42">
-        <v>0.756</v>
+        <v>0.743</v>
       </c>
       <c r="E42">
-        <v>0.632</v>
+        <v>0.639</v>
       </c>
       <c r="F42">
         <v>10</v>
       </c>
       <c r="G42">
-        <v>0.5339865278628292</v>
+        <v>0.5731781996325781</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1414,16 +1414,16 @@
         <v>19</v>
       </c>
       <c r="D43">
-        <v>0.786</v>
+        <v>0.765</v>
       </c>
       <c r="E43">
-        <v>0.64</v>
+        <v>0.648</v>
       </c>
       <c r="F43">
         <v>16</v>
       </c>
       <c r="G43">
-        <v>0.5278628291488059</v>
+        <v>0.5701163502755664</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1437,16 +1437,16 @@
         <v>19</v>
       </c>
       <c r="D44">
-        <v>0.804</v>
+        <v>0.783</v>
       </c>
       <c r="E44">
-        <v>0.644</v>
+        <v>0.654</v>
       </c>
       <c r="F44">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G44">
-        <v>0.5094917330067361</v>
+        <v>0.5820575627679119</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1460,16 +1460,16 @@
         <v>19</v>
       </c>
       <c r="D45">
-        <v>0.833</v>
+        <v>0.8080000000000001</v>
       </c>
       <c r="E45">
-        <v>0.645</v>
+        <v>0.656</v>
       </c>
       <c r="F45">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G45">
-        <v>0.4874464176362523</v>
+        <v>0.546846295162278</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1483,16 +1483,16 @@
         <v>19</v>
       </c>
       <c r="D46">
-        <v>0.769</v>
+        <v>0.752</v>
       </c>
       <c r="E46">
-        <v>0.641</v>
+        <v>0.644</v>
       </c>
       <c r="F46">
         <v>12</v>
       </c>
       <c r="G46">
-        <v>0.5379669320269442</v>
+        <v>0.5725658297611758</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1506,16 +1506,16 @@
         <v>19</v>
       </c>
       <c r="D47">
-        <v>0.802</v>
+        <v>0.778</v>
       </c>
       <c r="E47">
-        <v>0.644</v>
+        <v>0.649</v>
       </c>
       <c r="F47">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G47">
-        <v>0.518677281077771</v>
+        <v>0.5676668707899571</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1529,16 +1529,16 @@
         <v>19</v>
       </c>
       <c r="D48">
-        <v>0.822</v>
+        <v>0.797</v>
       </c>
       <c r="E48">
-        <v>0.646</v>
+        <v>0.657</v>
       </c>
       <c r="F48">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G48">
-        <v>0.484996938150643</v>
+        <v>0.5639926515615432</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1552,16 +1552,16 @@
         <v>19</v>
       </c>
       <c r="D49">
-        <v>0.849</v>
+        <v>0.819</v>
       </c>
       <c r="E49">
-        <v>0.648</v>
+        <v>0.659</v>
       </c>
       <c r="F49">
         <v>31</v>
       </c>
       <c r="G49">
-        <v>0.4611145131659523</v>
+        <v>0.533680342927128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>